<commit_message>
Add Incomplete Visit Feature (domain, hdsform, and functionality)
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/incomplete_form.xlsx
+++ b/app/src/main/res/raw/incomplete_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17670" tabRatio="500"/>
+    <workbookView windowWidth="23385" windowHeight="10410" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="78">
   <si>
     <t>group</t>
   </si>
@@ -151,16 +151,19 @@
     <t>2.1. Reason for not being visited</t>
   </si>
   <si>
-    <t>2.3. Motivo para não ter sido visitado</t>
+    <t>2.1. Motivo para não ter sido visitado</t>
   </si>
   <si>
     <t>reasonOther</t>
   </si>
   <si>
-    <t>2.3.1. Specify the reason for not being visited</t>
-  </si>
-  <si>
-    <t>2.3.1. Especifique o motivo para não ter sido visitado</t>
+    <t>2.2. Specify the reason for not being visited</t>
+  </si>
+  <si>
+    <t>2.2. Especifique o motivo para não ter sido visitado</t>
+  </si>
+  <si>
+    <t>${reason} = 'OTHER'</t>
   </si>
   <si>
     <t>collected</t>
@@ -175,7 +178,7 @@
     <t>3.1. Collected By Fieldworker</t>
   </si>
   <si>
-    <t>4.1. Códido do Inquiridor</t>
+    <t>3.1. Códido do Inquiridor</t>
   </si>
   <si>
     <t>collectedDate</t>
@@ -187,46 +190,82 @@
     <t>3.2. Collected Date</t>
   </si>
   <si>
-    <t>4.2. Data da Visita</t>
-  </si>
-  <si>
-    <t>modules</t>
-  </si>
-  <si>
-    <t>Access Granted to Modules</t>
-  </si>
-  <si>
-    <t>Acesso permitido aos Módulos</t>
+    <t>3.2. Data da Visita</t>
   </si>
   <si>
     <t>value</t>
   </si>
   <si>
+    <t>UNAVAILABLE_TODAY</t>
+  </si>
+  <si>
     <t>Not available today</t>
   </si>
   <si>
-    <t>N</t>
+    <t>Não esta disponível hoje</t>
+  </si>
+  <si>
+    <t>UNAVAILABLE_ROUND</t>
   </si>
   <si>
     <t xml:space="preserve">Not available this round (temporarily out of the area – away for school, work)  </t>
   </si>
   <si>
+    <t>Não esta disponível nesta ronda (temporariamente fora, pelos estudos, trabalho, etc)</t>
+  </si>
+  <si>
+    <t>UNWILLING</t>
+  </si>
+  <si>
     <t>Unwilling to participate this round</t>
   </si>
   <si>
+    <t>Não deseja participar nesta ronda</t>
+  </si>
+  <si>
+    <t>HOSPITALIZED</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hospitalized </t>
   </si>
   <si>
+    <t>Hospitalizado</t>
+  </si>
+  <si>
+    <t>RELOCATED</t>
+  </si>
+  <si>
     <t>Permanently relocated out of the study area</t>
   </si>
   <si>
+    <t>Emigrou para fora da area de estudo</t>
+  </si>
+  <si>
+    <t>WITHDREW</t>
+  </si>
+  <si>
     <t xml:space="preserve">Withdrew consent </t>
   </si>
   <si>
+    <t>Rejeitou/Retirou o consentimento</t>
+  </si>
+  <si>
+    <t>DEAD</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dead  </t>
   </si>
   <si>
+    <t>Morto</t>
+  </si>
+  <si>
+    <t>OTHER</t>
+  </si>
+  <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>Outra</t>
   </si>
   <si>
     <t>form_id</t>
@@ -252,10 +291,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -281,10 +320,101 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -296,9 +426,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,121 +463,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -458,6 +497,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -470,48 +521,150 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -519,120 +672,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -650,7 +689,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -670,17 +709,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -700,22 +733,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -743,155 +771,166 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -914,9 +953,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1239,10 +1275,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I8" sqref="B8:I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1301,7 +1337,7 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="N1" s="11" t="s">
         <v>13</v>
       </c>
       <c r="O1" t="s">
@@ -1336,7 +1372,7 @@
       <c r="M2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N2" s="12"/>
+      <c r="N2" s="11"/>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1" t="s">
@@ -1354,8 +1390,8 @@
       <c r="I3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
       <c r="L3" t="b">
         <v>1</v>
       </c>
@@ -1379,8 +1415,8 @@
       <c r="I4" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
       <c r="L4" t="b">
         <v>1</v>
       </c>
@@ -1404,8 +1440,8 @@
       <c r="I5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
       <c r="L5" t="b">
         <v>1</v>
       </c>
@@ -1413,7 +1449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:12">
       <c r="A6" s="1"/>
       <c r="D6" t="s">
         <v>29</v>
@@ -1421,7 +1457,7 @@
       <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H6" t="s">
@@ -1430,16 +1466,13 @@
       <c r="I6" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
       <c r="L6" t="b">
         <v>1</v>
       </c>
-      <c r="M6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1"/>
       <c r="D7" t="s">
         <v>34</v>
@@ -1453,35 +1486,36 @@
       <c r="I7" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
       <c r="L7" t="b">
         <v>1</v>
       </c>
-      <c r="M7" t="b">
-        <v>1</v>
+      <c r="M7"/>
+      <c r="N7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
       <c r="L8" t="b">
         <v>1</v>
       </c>
@@ -1491,22 +1525,22 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I9" t="s">
-        <v>45</v>
-      </c>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
+        <v>46</v>
+      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
       <c r="L9" t="b">
         <v>1</v>
       </c>
@@ -1514,45 +1548,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I10" t="s">
-        <v>48</v>
-      </c>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" t="b">
-        <v>1</v>
-      </c>
-      <c r="M10" t="b">
-        <v>1</v>
-      </c>
+    <row r="10" spans="1:11">
+      <c r="A10" s="1"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="1"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="1"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:1">
       <c r="A13" s="1"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="1"/>
@@ -1586,9 +1598,6 @@
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.39375" footer="0.39375"/>
@@ -1603,15 +1612,15 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="12.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="12.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="66.8380952380952" customWidth="1"/>
-    <col min="4" max="4" width="18.2857142857143" customWidth="1"/>
+    <col min="2" max="2" width="21.7142857142857" customWidth="1"/>
+    <col min="3" max="3" width="54.0571428571429" customWidth="1"/>
+    <col min="4" max="4" width="79.4285714285714" customWidth="1"/>
     <col min="5" max="5" width="13.1428571428571" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1620,7 +1629,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>7</v>
@@ -1636,14 +1645,14 @@
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="3">
-        <v>1</v>
+      <c r="B2" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="E2" s="2"/>
     </row>
@@ -1651,87 +1660,101 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="3">
-        <v>2</v>
+      <c r="B3" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="3">
-        <v>3</v>
+      <c r="B4" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="4">
-        <v>4</v>
+      <c r="B5" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="5"/>
+        <v>58</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="4">
-        <v>5</v>
+      <c r="B6" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" s="5"/>
+        <v>61</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="4">
-        <v>6</v>
+      <c r="B7" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>64</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="4">
-        <v>7</v>
+      <c r="B8" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="5"/>
+        <v>67</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="4">
-        <v>66</v>
+      <c r="B9" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="6"/>
@@ -1776,24 +1799,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Add more questions to VisitForm - check if visit is possible or not - Allow data collection with a non-resident respondent - Add Household and Member Status
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/incomplete_form.xlsx
+++ b/app/src/main/res/raw/incomplete_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27795" windowHeight="12270" tabRatio="500"/>
+    <workbookView windowWidth="25740" windowHeight="9840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -372,10 +372,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -396,6 +396,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -404,9 +412,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -418,6 +434,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -427,7 +480,29 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -435,14 +510,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -456,92 +539,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -573,13 +573,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,67 +663,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -663,43 +741,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -711,49 +753,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -844,6 +844,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -863,16 +872,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -892,41 +907,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -941,151 +921,171 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1464,7 +1464,7 @@
   <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="A8" sqref="$A8:$XFD12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
@@ -1930,14 +1930,14 @@
   <sheetPr/>
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView zoomScale="94" zoomScaleNormal="94" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.18095238095238" defaultRowHeight="12.75" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="12.5428571428571" customWidth="1"/>
-    <col min="2" max="2" width="21.7238095238095" customWidth="1"/>
+    <col min="2" max="2" width="23.4285714285714" customWidth="1"/>
     <col min="3" max="3" width="54" customWidth="1"/>
     <col min="4" max="4" width="79.4571428571429" customWidth="1"/>
     <col min="5" max="5" width="48.3619047619048" customWidth="1"/>

</xml_diff>